<commit_message>
Réalisation ACP et début description résultats.
</commit_message>
<xml_diff>
--- a/Analyse_flo_pedo_gestion/Data_flo_pedo_gestion.xlsx
+++ b/Analyse_flo_pedo_gestion/Data_flo_pedo_gestion.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\typha\OneDrive - umontpellier.fr\Documents\UM\FIRE\FIRE\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\typha\OneDrive - umontpellier.fr\Documents\UM\FIRE\Analyse_flo_pédologie_gestion\Analyse_flo_pedo_gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE87A164-1B29-4116-A051-272CDF1BC688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6234A1-B318-4AA7-9490-80FA069DC5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D94F8178-F691-4489-B0BB-8A12974AB300}"/>
   </bookViews>
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB364B25-869E-4B3D-BB65-9D0C1EDCA3A6}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1652,9 +1652,7 @@
       <c r="W14" s="6"/>
       <c r="X14" s="6"/>
       <c r="Y14" s="6"/>
-      <c r="Z14" s="5">
-        <v>1</v>
-      </c>
+      <c r="Z14" s="5"/>
     </row>
     <row r="15" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6"/>

</xml_diff>